<commit_message>
Added a few descriptions and titles of T.C. module Project history
</commit_message>
<xml_diff>
--- a/JAT Docs.xlsx
+++ b/JAT Docs.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="3"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Test Plan" sheetId="4" r:id="rId1"/>
@@ -18,10 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="39">
-  <si>
-    <t>Funcionalidades</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="40">
   <si>
     <t>Descripcion</t>
   </si>
@@ -144,6 +141,12 @@
   </si>
   <si>
     <t>Pasos para recrear el Bug</t>
+  </si>
+  <si>
+    <t>Feature</t>
+  </si>
+  <si>
+    <t>Funcionalidad</t>
   </si>
 </sst>
 </file>
@@ -339,7 +342,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -359,85 +362,94 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -449,12 +461,15 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -496,7 +511,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -531,7 +546,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -746,7 +761,7 @@
       <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -760,7 +775,7 @@
       <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="20.85546875" customWidth="1"/>
     <col min="3" max="3" width="34" customWidth="1"/>
@@ -770,146 +785,146 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="31" t="s">
+      <c r="B3" s="23" t="s">
+        <v>20</v>
+      </c>
+      <c r="C3" s="21" t="s">
+        <v>22</v>
+      </c>
+      <c r="D3" s="25" t="s">
+        <v>23</v>
+      </c>
+      <c r="E3" s="26"/>
+      <c r="F3" s="27"/>
+      <c r="G3" s="21" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="4" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B4" s="24"/>
+      <c r="C4" s="22"/>
+      <c r="D4" s="15"/>
+      <c r="E4" s="16"/>
+      <c r="F4" s="14"/>
+      <c r="G4" s="22"/>
+    </row>
+    <row r="5" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B5" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="C3" s="29" t="s">
-        <v>23</v>
-      </c>
-      <c r="D3" s="25" t="s">
+      <c r="C5" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="D5" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="E3" s="33"/>
-      <c r="F3" s="26"/>
-      <c r="G3" s="29" t="s">
+      <c r="E5" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="F5" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="G5" s="13" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="4" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B4" s="32"/>
-      <c r="C4" s="30"/>
-      <c r="D4" s="27"/>
-      <c r="E4" s="28"/>
-      <c r="F4" s="21"/>
-      <c r="G4" s="30"/>
-    </row>
-    <row r="5" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B5" s="20" t="s">
-        <v>22</v>
-      </c>
-      <c r="C5" s="20" t="s">
+    <row r="6" spans="2:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="B6" s="13"/>
+      <c r="C6" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="D5" s="22" t="s">
-        <v>25</v>
-      </c>
-      <c r="E5" s="20" t="s">
+      <c r="D6" s="19"/>
+      <c r="E6" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="F5" s="34" t="s">
+      <c r="F6" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="G5" s="20" t="s">
+      <c r="G6" s="13"/>
+    </row>
+    <row r="7" spans="2:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="B7" s="13"/>
+      <c r="C7" s="13"/>
+      <c r="D7" s="19"/>
+      <c r="E7" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="G7" s="13"/>
+    </row>
+    <row r="8" spans="2:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="B8" s="13"/>
+      <c r="C8" s="13"/>
+      <c r="D8" s="20"/>
+      <c r="E8" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="G8" s="13"/>
+    </row>
+    <row r="9" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B9" s="13"/>
+      <c r="C9" s="13"/>
+      <c r="D9" s="6" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="6" spans="2:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="B6" s="20"/>
-      <c r="C6" s="20" t="s">
-        <v>20</v>
-      </c>
-      <c r="D6" s="23"/>
-      <c r="E6" s="20" t="s">
-        <v>27</v>
-      </c>
-      <c r="F6" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="G6" s="20"/>
-    </row>
-    <row r="7" spans="2:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="B7" s="20"/>
-      <c r="C7" s="20"/>
-      <c r="D7" s="23"/>
-      <c r="E7" s="20" t="s">
-        <v>28</v>
-      </c>
-      <c r="F7" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="G7" s="20"/>
-    </row>
-    <row r="8" spans="2:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="B8" s="20"/>
-      <c r="C8" s="20"/>
-      <c r="D8" s="24"/>
-      <c r="E8" s="20" t="s">
-        <v>29</v>
-      </c>
-      <c r="F8" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="G8" s="20"/>
-    </row>
-    <row r="9" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B9" s="20"/>
-      <c r="C9" s="20"/>
-      <c r="D9" s="6" t="s">
+      <c r="E9" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="E9" s="20" t="s">
-        <v>33</v>
-      </c>
-      <c r="F9" s="20"/>
-      <c r="G9" s="20"/>
+      <c r="F9" s="13"/>
+      <c r="G9" s="13"/>
     </row>
     <row r="10" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B10" s="20"/>
-      <c r="C10" s="20"/>
-      <c r="D10" s="20"/>
-      <c r="E10" s="20"/>
-      <c r="F10" s="20"/>
-      <c r="G10" s="20"/>
+      <c r="B10" s="13"/>
+      <c r="C10" s="13"/>
+      <c r="D10" s="13"/>
+      <c r="E10" s="13"/>
+      <c r="F10" s="13"/>
+      <c r="G10" s="13"/>
     </row>
     <row r="11" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B11" s="20"/>
-      <c r="C11" s="20"/>
-      <c r="D11" s="20"/>
-      <c r="E11" s="20"/>
-      <c r="F11" s="20"/>
-      <c r="G11" s="20"/>
+      <c r="B11" s="13"/>
+      <c r="C11" s="13"/>
+      <c r="D11" s="13"/>
+      <c r="E11" s="13"/>
+      <c r="F11" s="13"/>
+      <c r="G11" s="13"/>
     </row>
     <row r="12" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B12" s="20"/>
-      <c r="C12" s="20"/>
-      <c r="D12" s="20"/>
-      <c r="E12" s="20"/>
-      <c r="F12" s="20"/>
-      <c r="G12" s="20"/>
+      <c r="B12" s="13"/>
+      <c r="C12" s="13"/>
+      <c r="D12" s="13"/>
+      <c r="E12" s="13"/>
+      <c r="F12" s="13"/>
+      <c r="G12" s="13"/>
     </row>
     <row r="13" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B13" s="20"/>
-      <c r="C13" s="20"/>
-      <c r="D13" s="20"/>
-      <c r="E13" s="20"/>
-      <c r="F13" s="20"/>
-      <c r="G13" s="20"/>
+      <c r="B13" s="13"/>
+      <c r="C13" s="13"/>
+      <c r="D13" s="13"/>
+      <c r="E13" s="13"/>
+      <c r="F13" s="13"/>
+      <c r="G13" s="13"/>
     </row>
     <row r="14" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B14" s="20"/>
-      <c r="C14" s="20"/>
-      <c r="D14" s="20"/>
-      <c r="E14" s="20"/>
-      <c r="F14" s="20"/>
-      <c r="G14" s="20"/>
+      <c r="B14" s="13"/>
+      <c r="C14" s="13"/>
+      <c r="D14" s="13"/>
+      <c r="E14" s="13"/>
+      <c r="F14" s="13"/>
+      <c r="G14" s="13"/>
     </row>
     <row r="15" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B15" s="20"/>
-      <c r="C15" s="20"/>
-      <c r="D15" s="20"/>
-      <c r="E15" s="20"/>
-      <c r="F15" s="20"/>
-      <c r="G15" s="20"/>
+      <c r="B15" s="13"/>
+      <c r="C15" s="13"/>
+      <c r="D15" s="13"/>
+      <c r="E15" s="13"/>
+      <c r="F15" s="13"/>
+      <c r="G15" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -925,196 +940,219 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:E23"/>
+  <dimension ref="A2:F23"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7:B22"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="23.85546875" style="1" customWidth="1"/>
     <col min="2" max="2" width="18.42578125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="43.140625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="37.28515625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="41.5703125" style="1" customWidth="1"/>
-    <col min="6" max="16384" width="9.140625" style="1"/>
+    <col min="3" max="4" width="43.140625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="37.28515625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="41.5703125" style="1" customWidth="1"/>
+    <col min="7" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B2" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="180" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="28" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" s="29" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="35" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3" s="7"/>
+      <c r="E3" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="F3" s="9" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4" s="28"/>
+      <c r="B4" s="30"/>
+      <c r="C4" s="36"/>
+      <c r="D4" s="10"/>
+      <c r="E4" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="F4" s="11"/>
+    </row>
+    <row r="5" spans="1:6" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="28"/>
+      <c r="B5" s="30"/>
+      <c r="C5" s="36"/>
+      <c r="D5" s="10"/>
+      <c r="E5" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="F5" s="11"/>
+    </row>
+    <row r="6" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A6" s="28"/>
+      <c r="B6" s="31"/>
+      <c r="C6" s="37"/>
+      <c r="D6" s="12"/>
+      <c r="E6" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="F6" s="11"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B7" s="32" t="s">
         <v>9</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="E2" s="5" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" ht="180" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="16" t="s">
-        <v>15</v>
-      </c>
-      <c r="B3" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="D3" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="E3" s="10" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="16"/>
-      <c r="B4" s="11"/>
-      <c r="C4" s="12"/>
-      <c r="D4" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="E4" s="13"/>
-    </row>
-    <row r="5" spans="1:5" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="16"/>
-      <c r="B5" s="11"/>
-      <c r="C5" s="12"/>
-      <c r="D5" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="E5" s="13"/>
-    </row>
-    <row r="6" spans="1:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="A6" s="16"/>
-      <c r="B6" s="14"/>
-      <c r="C6" s="15"/>
-      <c r="D6" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="E6" s="13"/>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B7" s="17" t="s">
-        <v>10</v>
       </c>
       <c r="C7" s="4"/>
       <c r="D7" s="4"/>
       <c r="E7" s="4"/>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B8" s="17"/>
+      <c r="F7" s="4"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B8" s="32"/>
       <c r="C8" s="4"/>
       <c r="D8" s="4"/>
       <c r="E8" s="4"/>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B9" s="17"/>
+      <c r="F8" s="4"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B9" s="32"/>
       <c r="C9" s="4"/>
       <c r="D9" s="4"/>
       <c r="E9" s="4"/>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B10" s="17"/>
+      <c r="F9" s="4"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B10" s="32"/>
       <c r="C10" s="4"/>
       <c r="D10" s="4"/>
       <c r="E10" s="4"/>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B11" s="17"/>
+      <c r="F10" s="4"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B11" s="32"/>
       <c r="C11" s="4"/>
       <c r="D11" s="4"/>
       <c r="E11" s="4"/>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B12" s="17" t="s">
-        <v>11</v>
+      <c r="F11" s="4"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B12" s="32" t="s">
+        <v>10</v>
       </c>
       <c r="C12" s="4"/>
       <c r="D12" s="4"/>
       <c r="E12" s="4"/>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B13" s="17"/>
+      <c r="F12" s="4"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B13" s="32"/>
       <c r="C13" s="4"/>
       <c r="D13" s="4"/>
       <c r="E13" s="4"/>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B14" s="17"/>
+      <c r="F13" s="4"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B14" s="32"/>
       <c r="C14" s="4"/>
       <c r="D14" s="4"/>
       <c r="E14" s="4"/>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B15" s="17"/>
+      <c r="F14" s="4"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B15" s="32"/>
       <c r="C15" s="4"/>
       <c r="D15" s="4"/>
       <c r="E15" s="4"/>
-    </row>
-    <row r="16" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="18" t="s">
-        <v>12</v>
+      <c r="F15" s="4"/>
+    </row>
+    <row r="16" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B16" s="33" t="s">
+        <v>11</v>
       </c>
       <c r="C16" s="4"/>
       <c r="D16" s="4"/>
       <c r="E16" s="4"/>
-    </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B17" s="18"/>
+      <c r="F16" s="4"/>
+    </row>
+    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B17" s="33"/>
       <c r="C17" s="4"/>
       <c r="D17" s="4"/>
       <c r="E17" s="4"/>
-    </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B18" s="18"/>
+      <c r="F17" s="4"/>
+    </row>
+    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B18" s="33"/>
       <c r="C18" s="4"/>
       <c r="D18" s="4"/>
       <c r="E18" s="4"/>
-    </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B19" s="19" t="s">
-        <v>13</v>
+      <c r="F18" s="4"/>
+    </row>
+    <row r="19" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B19" s="34" t="s">
+        <v>12</v>
       </c>
       <c r="C19" s="4"/>
       <c r="D19" s="4"/>
       <c r="E19" s="4"/>
-    </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B20" s="19"/>
+      <c r="F19" s="4"/>
+    </row>
+    <row r="20" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B20" s="34"/>
       <c r="C20" s="4"/>
       <c r="D20" s="4"/>
       <c r="E20" s="4"/>
-    </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B21" s="19"/>
+      <c r="F20" s="4"/>
+    </row>
+    <row r="21" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B21" s="34"/>
       <c r="C21" s="4"/>
       <c r="D21" s="4"/>
       <c r="E21" s="4"/>
-    </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B22" s="19"/>
+      <c r="F21" s="4"/>
+    </row>
+    <row r="22" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B22" s="34"/>
       <c r="C22" s="4"/>
       <c r="D22" s="4"/>
       <c r="E22" s="4"/>
-    </row>
-    <row r="23" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F22" s="4"/>
+    </row>
+    <row r="23" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B23" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="7">
+    <mergeCell ref="B19:B22"/>
+    <mergeCell ref="C3:C6"/>
     <mergeCell ref="A3:A6"/>
     <mergeCell ref="B3:B6"/>
     <mergeCell ref="B7:B11"/>
     <mergeCell ref="B12:B15"/>
     <mergeCell ref="B16:B18"/>
-    <mergeCell ref="B19:B22"/>
-    <mergeCell ref="C3:C6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1125,11 +1163,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:G18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="16.5703125" customWidth="1"/>
     <col min="3" max="3" width="18.5703125" customWidth="1"/>
@@ -1141,159 +1179,159 @@
   <sheetData>
     <row r="2" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B2" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="3" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B3" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="D2" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="E2" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="F2" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="G2" s="5" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="3" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B3" s="17" t="s">
+      <c r="C3" s="13"/>
+      <c r="D3" s="13"/>
+      <c r="E3" s="13"/>
+      <c r="F3" s="13"/>
+      <c r="G3" s="13"/>
+    </row>
+    <row r="4" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B4" s="32"/>
+      <c r="C4" s="13"/>
+      <c r="D4" s="13"/>
+      <c r="E4" s="13"/>
+      <c r="F4" s="13"/>
+      <c r="G4" s="13"/>
+    </row>
+    <row r="5" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B5" s="32"/>
+      <c r="C5" s="13"/>
+      <c r="D5" s="13"/>
+      <c r="E5" s="13"/>
+      <c r="F5" s="13"/>
+      <c r="G5" s="13"/>
+    </row>
+    <row r="6" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B6" s="32"/>
+      <c r="C6" s="13"/>
+      <c r="D6" s="13"/>
+      <c r="E6" s="13"/>
+      <c r="F6" s="13"/>
+      <c r="G6" s="13"/>
+    </row>
+    <row r="7" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B7" s="32"/>
+      <c r="C7" s="13"/>
+      <c r="D7" s="13"/>
+      <c r="E7" s="13"/>
+      <c r="F7" s="13"/>
+      <c r="G7" s="13"/>
+    </row>
+    <row r="8" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B8" s="32" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="20"/>
-      <c r="D3" s="20"/>
-      <c r="E3" s="20"/>
-      <c r="F3" s="20"/>
-      <c r="G3" s="20"/>
-    </row>
-    <row r="4" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B4" s="17"/>
-      <c r="C4" s="20"/>
-      <c r="D4" s="20"/>
-      <c r="E4" s="20"/>
-      <c r="F4" s="20"/>
-      <c r="G4" s="20"/>
-    </row>
-    <row r="5" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B5" s="17"/>
-      <c r="C5" s="20"/>
-      <c r="D5" s="20"/>
-      <c r="E5" s="20"/>
-      <c r="F5" s="20"/>
-      <c r="G5" s="20"/>
-    </row>
-    <row r="6" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B6" s="17"/>
-      <c r="C6" s="20"/>
-      <c r="D6" s="20"/>
-      <c r="E6" s="20"/>
-      <c r="F6" s="20"/>
-      <c r="G6" s="20"/>
-    </row>
-    <row r="7" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B7" s="17"/>
-      <c r="C7" s="20"/>
-      <c r="D7" s="20"/>
-      <c r="E7" s="20"/>
-      <c r="F7" s="20"/>
-      <c r="G7" s="20"/>
-    </row>
-    <row r="8" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B8" s="17" t="s">
+      <c r="C8" s="13"/>
+      <c r="D8" s="13"/>
+      <c r="E8" s="13"/>
+      <c r="F8" s="13"/>
+      <c r="G8" s="13"/>
+    </row>
+    <row r="9" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B9" s="32"/>
+      <c r="C9" s="13"/>
+      <c r="D9" s="13"/>
+      <c r="E9" s="13"/>
+      <c r="F9" s="13"/>
+      <c r="G9" s="13"/>
+    </row>
+    <row r="10" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B10" s="32"/>
+      <c r="C10" s="13"/>
+      <c r="D10" s="13"/>
+      <c r="E10" s="13"/>
+      <c r="F10" s="13"/>
+      <c r="G10" s="13"/>
+    </row>
+    <row r="11" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B11" s="32"/>
+      <c r="C11" s="13"/>
+      <c r="D11" s="13"/>
+      <c r="E11" s="13"/>
+      <c r="F11" s="13"/>
+      <c r="G11" s="13"/>
+    </row>
+    <row r="12" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B12" s="33" t="s">
         <v>11</v>
       </c>
-      <c r="C8" s="20"/>
-      <c r="D8" s="20"/>
-      <c r="E8" s="20"/>
-      <c r="F8" s="20"/>
-      <c r="G8" s="20"/>
-    </row>
-    <row r="9" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B9" s="17"/>
-      <c r="C9" s="20"/>
-      <c r="D9" s="20"/>
-      <c r="E9" s="20"/>
-      <c r="F9" s="20"/>
-      <c r="G9" s="20"/>
-    </row>
-    <row r="10" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B10" s="17"/>
-      <c r="C10" s="20"/>
-      <c r="D10" s="20"/>
-      <c r="E10" s="20"/>
-      <c r="F10" s="20"/>
-      <c r="G10" s="20"/>
-    </row>
-    <row r="11" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B11" s="17"/>
-      <c r="C11" s="20"/>
-      <c r="D11" s="20"/>
-      <c r="E11" s="20"/>
-      <c r="F11" s="20"/>
-      <c r="G11" s="20"/>
-    </row>
-    <row r="12" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B12" s="18" t="s">
+      <c r="C12" s="13"/>
+      <c r="D12" s="13"/>
+      <c r="E12" s="13"/>
+      <c r="F12" s="13"/>
+      <c r="G12" s="13"/>
+    </row>
+    <row r="13" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B13" s="33"/>
+      <c r="C13" s="13"/>
+      <c r="D13" s="13"/>
+      <c r="E13" s="13"/>
+      <c r="F13" s="13"/>
+      <c r="G13" s="13"/>
+    </row>
+    <row r="14" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B14" s="33"/>
+      <c r="C14" s="13"/>
+      <c r="D14" s="13"/>
+      <c r="E14" s="13"/>
+      <c r="F14" s="13"/>
+      <c r="G14" s="13"/>
+    </row>
+    <row r="15" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B15" s="34" t="s">
         <v>12</v>
       </c>
-      <c r="C12" s="20"/>
-      <c r="D12" s="20"/>
-      <c r="E12" s="20"/>
-      <c r="F12" s="20"/>
-      <c r="G12" s="20"/>
-    </row>
-    <row r="13" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B13" s="18"/>
-      <c r="C13" s="20"/>
-      <c r="D13" s="20"/>
-      <c r="E13" s="20"/>
-      <c r="F13" s="20"/>
-      <c r="G13" s="20"/>
-    </row>
-    <row r="14" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B14" s="18"/>
-      <c r="C14" s="20"/>
-      <c r="D14" s="20"/>
-      <c r="E14" s="20"/>
-      <c r="F14" s="20"/>
-      <c r="G14" s="20"/>
-    </row>
-    <row r="15" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B15" s="19" t="s">
-        <v>13</v>
-      </c>
-      <c r="C15" s="20"/>
-      <c r="D15" s="20"/>
-      <c r="E15" s="20"/>
-      <c r="F15" s="20"/>
-      <c r="G15" s="20"/>
+      <c r="C15" s="13"/>
+      <c r="D15" s="13"/>
+      <c r="E15" s="13"/>
+      <c r="F15" s="13"/>
+      <c r="G15" s="13"/>
     </row>
     <row r="16" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B16" s="19"/>
-      <c r="C16" s="20"/>
-      <c r="D16" s="20"/>
-      <c r="E16" s="20"/>
-      <c r="F16" s="20"/>
-      <c r="G16" s="20"/>
+      <c r="B16" s="34"/>
+      <c r="C16" s="13"/>
+      <c r="D16" s="13"/>
+      <c r="E16" s="13"/>
+      <c r="F16" s="13"/>
+      <c r="G16" s="13"/>
     </row>
     <row r="17" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B17" s="19"/>
-      <c r="C17" s="20"/>
-      <c r="D17" s="20"/>
-      <c r="E17" s="20"/>
-      <c r="F17" s="20"/>
-      <c r="G17" s="20"/>
+      <c r="B17" s="34"/>
+      <c r="C17" s="13"/>
+      <c r="D17" s="13"/>
+      <c r="E17" s="13"/>
+      <c r="F17" s="13"/>
+      <c r="G17" s="13"/>
     </row>
     <row r="18" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B18" s="19"/>
-      <c r="C18" s="20"/>
-      <c r="D18" s="20"/>
-      <c r="E18" s="20"/>
-      <c r="F18" s="20"/>
-      <c r="G18" s="20"/>
+      <c r="B18" s="34"/>
+      <c r="C18" s="13"/>
+      <c r="D18" s="13"/>
+      <c r="E18" s="13"/>
+      <c r="F18" s="13"/>
+      <c r="G18" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -1312,7 +1350,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>